<commit_message>
update proses kirim tagihan
</commit_message>
<xml_diff>
--- a/template/assets/static/Form_upload_tagihan.xlsx
+++ b/template/assets/static/Form_upload_tagihan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\kasir\template\assets\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F2D7E7-8DF9-45F5-B4CF-89AD8E44BE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA7089D-4141-4EDF-B7C5-B19A3A1C5002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{687E2A08-6BD6-41BF-A602-15326EBCB938}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>FORM UPLOAD SLIP GAJI</t>
   </si>
@@ -51,18 +51,6 @@
     <t>NOMINAL</t>
   </si>
   <si>
-    <t>NO. HP</t>
-  </si>
-  <si>
-    <t>6285236924510</t>
-  </si>
-  <si>
-    <t>6289682351413</t>
-  </si>
-  <si>
-    <t>6281358259349</t>
-  </si>
-  <si>
     <t>BRIVA</t>
   </si>
   <si>
@@ -94,6 +82,9 @@
   </si>
   <si>
     <t>567890123456</t>
+  </si>
+  <si>
+    <t>NIS</t>
   </si>
 </sst>
 </file>
@@ -181,11 +172,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,7 +495,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="E5" sqref="E5:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,22 +507,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -541,13 +532,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -555,85 +546,75 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3">
         <v>500000</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3">
         <v>750000</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D7" s="3">
         <v>600000</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3">
         <v>800000</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3">
         <v>550000</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="E9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>